<commit_message>
DPV v0.9 update - RDF, HTML
- The code and docs have been updated and versioned as v0.9
- Changelogs have been generated
- The releases have NOT been generated
- The Manchester syntax files have NOT been generated
- The remaining release tasks will be completed on coming WED/THU
</commit_message>
<xml_diff>
--- a/documentation-generator/vocab_csv/base.xlsx
+++ b/documentation-generator/vocab_csv/base.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="269">
   <si>
     <t>preffix</t>
   </si>
@@ -281,6 +281,15 @@
   </si>
   <si>
     <t>Vocabulary of EU's Fundamental Rights for DPV-OWL</t>
+  </si>
+  <si>
+    <t>dex</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/examples#</t>
+  </si>
+  <si>
+    <t>Examples for DPV and associated vocabularies</t>
   </si>
   <si>
     <t>dct</t>
@@ -1961,6 +1970,23 @@
         <v>73</v>
       </c>
     </row>
+    <row r="27">
+      <c r="A27" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="D27" s="8">
+        <v>44856.0</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="B2"/>
@@ -2012,8 +2038,9 @@
     <hyperlink r:id="rId47" ref="H25"/>
     <hyperlink r:id="rId48" ref="B26"/>
     <hyperlink r:id="rId49" ref="H26"/>
+    <hyperlink r:id="rId50" ref="B27"/>
   </hyperlinks>
-  <drawing r:id="rId50"/>
+  <drawing r:id="rId51"/>
 </worksheet>
 </file>
 
@@ -2059,13 +2086,13 @@
     </row>
     <row r="2">
       <c r="A2" s="14" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="D2" s="16"/>
       <c r="E2" s="16"/>
@@ -2089,13 +2116,13 @@
     </row>
     <row r="3">
       <c r="A3" s="17" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D3" s="16"/>
       <c r="E3" s="16"/>
@@ -2119,13 +2146,13 @@
     </row>
     <row r="4">
       <c r="A4" s="17" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D4" s="16"/>
       <c r="E4" s="16"/>
@@ -2149,13 +2176,13 @@
     </row>
     <row r="5">
       <c r="A5" s="17" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="D5" s="16"/>
       <c r="E5" s="16"/>
@@ -2179,13 +2206,13 @@
     </row>
     <row r="6">
       <c r="A6" s="17" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D6" s="16"/>
       <c r="E6" s="16"/>
@@ -2209,13 +2236,13 @@
     </row>
     <row r="7">
       <c r="A7" s="14" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="D7" s="16"/>
       <c r="E7" s="16"/>
@@ -2239,10 +2266,10 @@
     </row>
     <row r="8">
       <c r="A8" s="14" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C8" s="20" t="str">
         <f>HYPERLINK("https://www.specialprivacy.eu/images/documents/SPECIAL_D25_M21_V10.pdf","SPECIAL Log vocabulary cf. SPECIAL Deliverable D2.5")</f>
@@ -2270,13 +2297,13 @@
     </row>
     <row r="9">
       <c r="A9" s="14" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="D9" s="16"/>
       <c r="E9" s="16"/>
@@ -2300,13 +2327,13 @@
     </row>
     <row r="10">
       <c r="A10" s="14" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D10" s="16"/>
       <c r="E10" s="16"/>
@@ -2330,13 +2357,13 @@
     </row>
     <row r="11">
       <c r="A11" s="22" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="D11" s="16"/>
       <c r="E11" s="16"/>
@@ -2360,13 +2387,13 @@
     </row>
     <row r="12">
       <c r="A12" s="14" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="D12" s="16"/>
       <c r="E12" s="16"/>
@@ -2390,13 +2417,13 @@
     </row>
     <row r="13">
       <c r="A13" s="14" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="D13" s="16"/>
       <c r="E13" s="16"/>
@@ -2420,13 +2447,13 @@
     </row>
     <row r="14">
       <c r="A14" s="22" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="D14" s="16"/>
       <c r="E14" s="16"/>
@@ -2450,79 +2477,79 @@
     </row>
     <row r="15">
       <c r="A15" s="6" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="6" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="6" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="6" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="6" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="6" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="6" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -2577,66 +2604,66 @@
   <sheetData>
     <row r="1" ht="28.5" customHeight="1">
       <c r="A1" s="23" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="D1" s="23" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="E1" s="23" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="F1" s="23" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="G1" s="23" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="H1" s="23" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="I1" s="25" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="J1" s="26" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="L1" s="27" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="6" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -2650,13 +2677,13 @@
         <v>44139.0</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="P2" s="30"/>
       <c r="Q2" s="30"/>
@@ -2678,32 +2705,32 @@
     </row>
     <row r="3">
       <c r="A3" s="6" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="B3" s="31" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="F3" s="6"/>
       <c r="G3" s="6" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="J3" s="13" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="K3" s="8">
         <v>43560.0</v>
@@ -2712,13 +2739,13 @@
         <v>44580.0</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="O3" s="7" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="P3" s="30"/>
       <c r="Q3" s="30"/>
@@ -2740,30 +2767,30 @@
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="6" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="I4" s="30"/>
       <c r="J4" s="13" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="K4" s="8">
         <v>43560.0</v>
@@ -2772,13 +2799,13 @@
         <v>44139.0</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="O4" s="9" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="P4" s="30"/>
       <c r="Q4" s="30"/>
@@ -2800,30 +2827,30 @@
     </row>
     <row r="5">
       <c r="A5" s="6" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="6" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="I5" s="30"/>
       <c r="J5" s="6" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="K5" s="8">
         <v>43560.0</v>
@@ -2832,13 +2859,13 @@
         <v>44139.0</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="O5" s="9" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="P5" s="30"/>
       <c r="Q5" s="30"/>
@@ -2860,32 +2887,32 @@
     </row>
     <row r="6">
       <c r="A6" s="33" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="B6" s="34" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="6" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="I6" s="35" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="K6" s="8">
         <v>43560.0</v>
@@ -2894,13 +2921,13 @@
         <v>44139.0</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="O6" s="9" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="P6" s="30"/>
       <c r="Q6" s="30"/>
@@ -2922,19 +2949,19 @@
     </row>
     <row r="7">
       <c r="A7" s="33" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="B7" s="34" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="F7" s="30"/>
       <c r="G7" s="30"/>
@@ -2948,13 +2975,13 @@
         <v>44139.0</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="N7" s="6" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="O7" s="9" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="P7" s="30"/>
       <c r="Q7" s="30"/>
@@ -2976,25 +3003,25 @@
     </row>
     <row r="8">
       <c r="A8" s="33" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="B8" s="34" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="F8" s="30"/>
       <c r="G8" s="30"/>
       <c r="H8" s="30"/>
       <c r="I8" s="6" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="J8" s="6"/>
       <c r="K8" s="8">
@@ -3004,11 +3031,11 @@
         <v>44139.0</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="N8" s="30"/>
       <c r="O8" s="9" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="P8" s="30"/>
       <c r="Q8" s="30"/>
@@ -3030,28 +3057,28 @@
     </row>
     <row r="9">
       <c r="A9" s="33" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="B9" s="34" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="F9" s="30"/>
       <c r="G9" s="30"/>
       <c r="H9" s="30"/>
       <c r="I9" s="6" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="J9" s="36" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="K9" s="8">
         <v>43560.0</v>
@@ -3060,13 +3087,13 @@
         <v>44139.0</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="N9" s="6" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="O9" s="9" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="P9" s="30"/>
       <c r="Q9" s="30"/>
@@ -3088,28 +3115,28 @@
     </row>
     <row r="10">
       <c r="A10" s="33" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="B10" s="34" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="F10" s="30"/>
       <c r="G10" s="30"/>
       <c r="H10" s="30"/>
       <c r="I10" s="6" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="J10" s="36" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="K10" s="8">
         <v>43560.0</v>
@@ -3118,13 +3145,13 @@
         <v>44139.0</v>
       </c>
       <c r="M10" s="6" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="N10" s="6" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="O10" s="9" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="P10" s="30"/>
       <c r="Q10" s="30"/>
@@ -3146,25 +3173,25 @@
     </row>
     <row r="11">
       <c r="A11" s="37" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="B11" s="38" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="C11" s="37" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="F11" s="39"/>
       <c r="G11" s="39"/>
       <c r="H11" s="39"/>
       <c r="I11" s="37" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="J11" s="37"/>
       <c r="K11" s="40">
@@ -3172,13 +3199,13 @@
       </c>
       <c r="L11" s="40"/>
       <c r="M11" s="37" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="N11" s="37" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="O11" s="41" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="P11" s="39"/>
       <c r="Q11" s="39"/>
@@ -3200,25 +3227,25 @@
     </row>
     <row r="12">
       <c r="A12" s="37" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="B12" s="38" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="C12" s="37" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="D12" s="37" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="E12" s="37" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="F12" s="39"/>
       <c r="G12" s="39"/>
       <c r="H12" s="39"/>
       <c r="I12" s="37" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="J12" s="37"/>
       <c r="K12" s="40">
@@ -3226,13 +3253,13 @@
       </c>
       <c r="L12" s="40"/>
       <c r="M12" s="37" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="N12" s="37" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="O12" s="41" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="P12" s="39"/>
       <c r="Q12" s="39"/>
@@ -3254,25 +3281,25 @@
     </row>
     <row r="13">
       <c r="A13" s="42" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="C13" s="29" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="F13" s="30"/>
       <c r="G13" s="30"/>
       <c r="H13" s="30"/>
       <c r="I13" s="6" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="J13" s="6"/>
       <c r="K13" s="8">
@@ -3280,13 +3307,13 @@
       </c>
       <c r="L13" s="8"/>
       <c r="M13" s="42" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="N13" s="6" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="O13" s="36" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="P13" s="30"/>
       <c r="Q13" s="30"/>
@@ -6285,69 +6312,69 @@
   <sheetData>
     <row r="1" ht="28.5" customHeight="1">
       <c r="A1" s="23" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="D1" s="23" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="E1" s="23" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="F1" s="23" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="G1" s="23" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="H1" s="23" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="J1" s="26" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="33" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="E2" s="33" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="G2" s="30"/>
       <c r="H2" s="30"/>
@@ -6360,13 +6387,13 @@
         <v>44139.0</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="P2" s="30"/>
       <c r="Q2" s="30"/>
@@ -6384,23 +6411,23 @@
     </row>
     <row r="3">
       <c r="A3" s="33" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="E3" s="33" t="str">
         <f t="shared" ref="E3:E12" si="1">CONCATENATE("dpv:",RIGHT(A3,LEN(A3) - 3))</f>
         <v>dpv:DataSubject</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="G3" s="30"/>
       <c r="H3" s="30"/>
@@ -6413,13 +6440,13 @@
         <v>44139.0</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="O3" s="9" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="P3" s="30"/>
       <c r="Q3" s="30"/>
@@ -6437,23 +6464,23 @@
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="E4" s="30" t="str">
         <f t="shared" si="1"/>
         <v>dpv:LegalBasis</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="G4" s="30"/>
       <c r="H4" s="30"/>
@@ -6466,13 +6493,13 @@
         <v>44139.0</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="O4" s="9" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="P4" s="30"/>
       <c r="Q4" s="30"/>
@@ -6490,23 +6517,23 @@
     </row>
     <row r="5">
       <c r="A5" s="6" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="B5" s="31" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="E5" s="6" t="str">
         <f t="shared" si="1"/>
         <v>dpv:PersonalData</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="G5" s="30"/>
       <c r="H5" s="30"/>
@@ -6517,13 +6544,13 @@
       </c>
       <c r="L5" s="8"/>
       <c r="M5" s="6" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="O5" s="36" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="P5" s="30"/>
       <c r="Q5" s="30"/>
@@ -6541,23 +6568,23 @@
     </row>
     <row r="6">
       <c r="A6" s="6" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="E6" s="30" t="str">
         <f t="shared" si="1"/>
         <v>dpv:PersonalDataHandling</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="G6" s="30"/>
       <c r="H6" s="30"/>
@@ -6568,13 +6595,13 @@
       </c>
       <c r="L6" s="30"/>
       <c r="M6" s="6" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="O6" s="9" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="P6" s="30"/>
       <c r="Q6" s="30"/>
@@ -6592,29 +6619,29 @@
     </row>
     <row r="7">
       <c r="A7" s="6" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="B7" s="32" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="E7" s="6" t="str">
         <f t="shared" si="1"/>
         <v>dpv:Processing</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="G7" s="30"/>
       <c r="H7" s="30"/>
       <c r="I7" s="30"/>
       <c r="J7" s="6" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="K7" s="8">
         <v>43559.0</v>
@@ -6623,13 +6650,13 @@
         <v>44139.0</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="N7" s="6" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="O7" s="9" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="P7" s="30"/>
       <c r="Q7" s="30"/>
@@ -6647,29 +6674,29 @@
     </row>
     <row r="8">
       <c r="A8" s="6" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="B8" s="32" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="E8" s="6" t="str">
         <f t="shared" si="1"/>
         <v>dpv:Purpose</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="G8" s="30"/>
       <c r="H8" s="30"/>
       <c r="I8" s="30"/>
       <c r="J8" s="6" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="K8" s="8">
         <v>43559.0</v>
@@ -6678,13 +6705,13 @@
         <v>44139.0</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="N8" s="6" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="O8" s="9" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="P8" s="30"/>
       <c r="Q8" s="30"/>
@@ -6702,29 +6729,29 @@
     </row>
     <row r="9">
       <c r="A9" s="6" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="B9" s="32" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="E9" s="30" t="str">
         <f t="shared" si="1"/>
         <v>dpv:Recipient</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="G9" s="30"/>
       <c r="H9" s="30"/>
       <c r="I9" s="30"/>
       <c r="J9" s="6" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="K9" s="8">
         <v>43559.0</v>
@@ -6733,13 +6760,13 @@
         <v>44139.0</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="N9" s="6" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="O9" s="9" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="P9" s="30"/>
       <c r="Q9" s="30"/>
@@ -6757,23 +6784,23 @@
     </row>
     <row r="10">
       <c r="A10" s="37" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="C10" s="44" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="E10" s="39" t="str">
         <f t="shared" si="1"/>
         <v>dpv:Right</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="G10" s="39"/>
       <c r="H10" s="39"/>
@@ -6784,13 +6811,13 @@
       </c>
       <c r="L10" s="39"/>
       <c r="M10" s="37" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="N10" s="37" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="O10" s="41" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="P10" s="39"/>
       <c r="Q10" s="39"/>
@@ -6808,23 +6835,23 @@
     </row>
     <row r="11">
       <c r="A11" s="6" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="E11" s="30" t="str">
         <f t="shared" si="1"/>
         <v>dpv:Risk</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="G11" s="30"/>
       <c r="H11" s="30"/>
@@ -6835,13 +6862,13 @@
       </c>
       <c r="L11" s="30"/>
       <c r="M11" s="6" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="N11" s="6" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="O11" s="41" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="P11" s="30"/>
       <c r="Q11" s="30"/>
@@ -6859,23 +6886,23 @@
     </row>
     <row r="12">
       <c r="A12" s="6" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="B12" s="32" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="E12" s="30" t="str">
         <f t="shared" si="1"/>
         <v>dpv:TechnicalOrganisationalMeasure</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="G12" s="30"/>
       <c r="H12" s="30"/>
@@ -6888,13 +6915,13 @@
         <v>44139.0</v>
       </c>
       <c r="M12" s="6" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="N12" s="6" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="O12" s="9" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="P12" s="30"/>
       <c r="Q12" s="30"/>

</xml_diff>

<commit_message>
Adds Rights Exercise, and Updates/Fixes concepts
- Rights Exercise has concepts in main spec (rights) and dpv-gdpr
- Justifications.csv is a WIP spreadsheet that will host the
  justifications used for Rights Non-fulfilment and elsewhere
- New concepts / Modified concepts in DPV-PD, Context, Personal Data,
  Purposes (as part of refinements), and Status
- Note that this commit does not contain a changelog
</commit_message>
<xml_diff>
--- a/documentation-generator/vocab_csv/base.xlsx
+++ b/documentation-generator/vocab_csv/base.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="285">
   <si>
     <t>preffix</t>
   </si>
@@ -479,6 +479,15 @@
   </si>
   <si>
     <t>VANN: A vocabulary for annotating vocabulary descriptions</t>
+  </si>
+  <si>
+    <t>dcat</t>
+  </si>
+  <si>
+    <t>http://www.w3.org/ns/dcat#</t>
+  </si>
+  <si>
+    <t>Data Catalog Vocabulary (DCAT) - Version 2</t>
   </si>
   <si>
     <t>Term</t>
@@ -870,6 +879,27 @@
   </si>
   <si>
     <t>Indicates use or applicability of Technical or Organisational measure</t>
+  </si>
+  <si>
+    <t>dct:title</t>
+  </si>
+  <si>
+    <t>dct:description</t>
+  </si>
+  <si>
+    <t>dct:date</t>
+  </si>
+  <si>
+    <t>dct:isPartOf</t>
+  </si>
+  <si>
+    <t>dct:hasPart</t>
+  </si>
+  <si>
+    <t>dct:identifier</t>
+  </si>
+  <si>
+    <t>dct:subject</t>
   </si>
 </sst>
 </file>
@@ -2602,6 +2632,17 @@
         <v>154</v>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>157</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="B2"/>
@@ -2624,8 +2665,9 @@
     <hyperlink r:id="rId18" ref="B19"/>
     <hyperlink r:id="rId19" ref="B20"/>
     <hyperlink r:id="rId20" ref="B21"/>
+    <hyperlink r:id="rId21" ref="B22"/>
   </hyperlinks>
-  <drawing r:id="rId21"/>
+  <drawing r:id="rId22"/>
 </worksheet>
 </file>
 
@@ -2654,66 +2696,66 @@
   <sheetData>
     <row r="1" ht="28.5" customHeight="1">
       <c r="A1" s="24" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="C1" s="25" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="D1" s="24" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="E1" s="24" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="F1" s="24" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="G1" s="24" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="H1" s="24" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="I1" s="26" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="J1" s="27" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="L1" s="28" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="6" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -2727,13 +2769,13 @@
         <v>44139.0</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="P2" s="31"/>
       <c r="Q2" s="31"/>
@@ -2755,32 +2797,32 @@
     </row>
     <row r="3">
       <c r="A3" s="6" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F3" s="6"/>
       <c r="G3" s="6" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="J3" s="13" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="K3" s="8">
         <v>43560.0</v>
@@ -2789,13 +2831,13 @@
         <v>44580.0</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="O3" s="7" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="P3" s="31"/>
       <c r="Q3" s="31"/>
@@ -2817,30 +2859,30 @@
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="6" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="I4" s="31"/>
       <c r="J4" s="13" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="K4" s="8">
         <v>43560.0</v>
@@ -2849,13 +2891,13 @@
         <v>44139.0</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="O4" s="9" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="P4" s="31"/>
       <c r="Q4" s="31"/>
@@ -2877,30 +2919,30 @@
     </row>
     <row r="5">
       <c r="A5" s="6" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="B5" s="33" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="6" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="I5" s="31"/>
       <c r="J5" s="6" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="K5" s="8">
         <v>43560.0</v>
@@ -2909,13 +2951,13 @@
         <v>44139.0</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="O5" s="9" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="P5" s="31"/>
       <c r="Q5" s="31"/>
@@ -2937,32 +2979,32 @@
     </row>
     <row r="6">
       <c r="A6" s="34" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="B6" s="35" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="6" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="I6" s="36" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="K6" s="8">
         <v>43560.0</v>
@@ -2971,13 +3013,13 @@
         <v>44139.0</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="O6" s="9" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="P6" s="31"/>
       <c r="Q6" s="31"/>
@@ -2999,19 +3041,19 @@
     </row>
     <row r="7">
       <c r="A7" s="34" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="B7" s="35" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="F7" s="31"/>
       <c r="G7" s="31"/>
@@ -3025,13 +3067,13 @@
         <v>44139.0</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="N7" s="6" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="O7" s="9" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="P7" s="31"/>
       <c r="Q7" s="31"/>
@@ -3053,25 +3095,25 @@
     </row>
     <row r="8">
       <c r="A8" s="34" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="B8" s="35" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="F8" s="31"/>
       <c r="G8" s="31"/>
       <c r="H8" s="31"/>
       <c r="I8" s="6" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="J8" s="6"/>
       <c r="K8" s="8">
@@ -3081,11 +3123,11 @@
         <v>44139.0</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="N8" s="31"/>
       <c r="O8" s="9" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="P8" s="31"/>
       <c r="Q8" s="31"/>
@@ -3107,28 +3149,28 @@
     </row>
     <row r="9">
       <c r="A9" s="34" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="B9" s="35" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F9" s="31"/>
       <c r="G9" s="31"/>
       <c r="H9" s="31"/>
       <c r="I9" s="6" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="J9" s="37" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="K9" s="8">
         <v>43560.0</v>
@@ -3137,13 +3179,13 @@
         <v>44139.0</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="N9" s="6" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="O9" s="9" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="P9" s="31"/>
       <c r="Q9" s="31"/>
@@ -3165,28 +3207,28 @@
     </row>
     <row r="10">
       <c r="A10" s="34" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="B10" s="35" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F10" s="31"/>
       <c r="G10" s="31"/>
       <c r="H10" s="31"/>
       <c r="I10" s="6" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="J10" s="37" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="K10" s="8">
         <v>43560.0</v>
@@ -3195,13 +3237,13 @@
         <v>44139.0</v>
       </c>
       <c r="M10" s="6" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="N10" s="6" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="O10" s="9" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="P10" s="31"/>
       <c r="Q10" s="31"/>
@@ -3223,25 +3265,25 @@
     </row>
     <row r="11">
       <c r="A11" s="38" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="B11" s="39" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="C11" s="38" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="F11" s="40"/>
       <c r="G11" s="40"/>
       <c r="H11" s="40"/>
       <c r="I11" s="38" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="J11" s="38"/>
       <c r="K11" s="41">
@@ -3249,13 +3291,13 @@
       </c>
       <c r="L11" s="41"/>
       <c r="M11" s="38" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="N11" s="38" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="O11" s="42" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="P11" s="40"/>
       <c r="Q11" s="40"/>
@@ -3277,25 +3319,25 @@
     </row>
     <row r="12">
       <c r="A12" s="38" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="B12" s="39" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="C12" s="38" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="D12" s="38" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="E12" s="38" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F12" s="40"/>
       <c r="G12" s="40"/>
       <c r="H12" s="40"/>
       <c r="I12" s="38" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="J12" s="38"/>
       <c r="K12" s="41">
@@ -3303,13 +3345,13 @@
       </c>
       <c r="L12" s="41"/>
       <c r="M12" s="38" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="N12" s="38" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="O12" s="42" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="P12" s="40"/>
       <c r="Q12" s="40"/>
@@ -3331,25 +3373,25 @@
     </row>
     <row r="13">
       <c r="A13" s="43" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="F13" s="31"/>
       <c r="G13" s="31"/>
       <c r="H13" s="31"/>
       <c r="I13" s="6" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="J13" s="6"/>
       <c r="K13" s="8">
@@ -3357,13 +3399,13 @@
       </c>
       <c r="L13" s="8"/>
       <c r="M13" s="43" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="N13" s="6" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="O13" s="37" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="P13" s="31"/>
       <c r="Q13" s="31"/>
@@ -6362,69 +6404,69 @@
   <sheetData>
     <row r="1" ht="28.5" customHeight="1">
       <c r="A1" s="24" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="C1" s="25" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="D1" s="24" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="E1" s="24" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="F1" s="24" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="G1" s="24" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="H1" s="24" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="J1" s="27" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="34" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="E2" s="34" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="G2" s="31"/>
       <c r="H2" s="31"/>
@@ -6437,13 +6479,13 @@
         <v>44139.0</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="P2" s="31"/>
       <c r="Q2" s="31"/>
@@ -6461,23 +6503,23 @@
     </row>
     <row r="3">
       <c r="A3" s="34" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="B3" s="35" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="E3" s="34" t="str">
         <f t="shared" ref="E3:E12" si="1">CONCATENATE("dpv:",RIGHT(A3,LEN(A3) - 3))</f>
         <v>dpv:DataSubject</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="G3" s="31"/>
       <c r="H3" s="31"/>
@@ -6490,13 +6532,13 @@
         <v>44139.0</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="O3" s="9" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="P3" s="31"/>
       <c r="Q3" s="31"/>
@@ -6514,23 +6556,23 @@
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="E4" s="31" t="str">
         <f t="shared" si="1"/>
         <v>dpv:LegalBasis</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="G4" s="31"/>
       <c r="H4" s="31"/>
@@ -6543,13 +6585,13 @@
         <v>44139.0</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="O4" s="9" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="P4" s="31"/>
       <c r="Q4" s="31"/>
@@ -6567,23 +6609,23 @@
     </row>
     <row r="5">
       <c r="A5" s="6" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="E5" s="6" t="str">
         <f t="shared" si="1"/>
         <v>dpv:PersonalData</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="G5" s="31"/>
       <c r="H5" s="31"/>
@@ -6594,13 +6636,13 @@
       </c>
       <c r="L5" s="8"/>
       <c r="M5" s="6" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="O5" s="37" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="P5" s="31"/>
       <c r="Q5" s="31"/>
@@ -6618,23 +6660,23 @@
     </row>
     <row r="6">
       <c r="A6" s="6" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="E6" s="31" t="str">
         <f t="shared" si="1"/>
         <v>dpv:PersonalDataHandling</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="G6" s="31"/>
       <c r="H6" s="31"/>
@@ -6645,13 +6687,13 @@
       </c>
       <c r="L6" s="31"/>
       <c r="M6" s="6" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="O6" s="9" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="P6" s="31"/>
       <c r="Q6" s="31"/>
@@ -6669,29 +6711,29 @@
     </row>
     <row r="7">
       <c r="A7" s="6" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="B7" s="33" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="E7" s="6" t="str">
         <f t="shared" si="1"/>
         <v>dpv:Processing</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="G7" s="31"/>
       <c r="H7" s="31"/>
       <c r="I7" s="31"/>
       <c r="J7" s="6" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="K7" s="8">
         <v>43559.0</v>
@@ -6700,13 +6742,13 @@
         <v>44139.0</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="N7" s="6" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="O7" s="9" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="P7" s="31"/>
       <c r="Q7" s="31"/>
@@ -6724,29 +6766,29 @@
     </row>
     <row r="8">
       <c r="A8" s="6" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="B8" s="33" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="E8" s="6" t="str">
         <f t="shared" si="1"/>
         <v>dpv:Purpose</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="G8" s="31"/>
       <c r="H8" s="31"/>
       <c r="I8" s="31"/>
       <c r="J8" s="6" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="K8" s="8">
         <v>43559.0</v>
@@ -6755,13 +6797,13 @@
         <v>44139.0</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="N8" s="6" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="O8" s="9" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="P8" s="31"/>
       <c r="Q8" s="31"/>
@@ -6779,29 +6821,29 @@
     </row>
     <row r="9">
       <c r="A9" s="6" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="B9" s="33" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="E9" s="31" t="str">
         <f t="shared" si="1"/>
         <v>dpv:Recipient</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="G9" s="31"/>
       <c r="H9" s="31"/>
       <c r="I9" s="31"/>
       <c r="J9" s="6" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="K9" s="8">
         <v>43559.0</v>
@@ -6810,13 +6852,13 @@
         <v>44139.0</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="N9" s="6" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="O9" s="9" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="P9" s="31"/>
       <c r="Q9" s="31"/>
@@ -6834,23 +6876,23 @@
     </row>
     <row r="10">
       <c r="A10" s="38" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="B10" s="38" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="C10" s="45" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="E10" s="40" t="str">
         <f t="shared" si="1"/>
         <v>dpv:Right</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="G10" s="40"/>
       <c r="H10" s="40"/>
@@ -6861,13 +6903,13 @@
       </c>
       <c r="L10" s="40"/>
       <c r="M10" s="38" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="N10" s="38" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="O10" s="42" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="P10" s="40"/>
       <c r="Q10" s="40"/>
@@ -6885,23 +6927,23 @@
     </row>
     <row r="11">
       <c r="A11" s="6" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="E11" s="31" t="str">
         <f t="shared" si="1"/>
         <v>dpv:Risk</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="G11" s="31"/>
       <c r="H11" s="31"/>
@@ -6912,13 +6954,13 @@
       </c>
       <c r="L11" s="31"/>
       <c r="M11" s="6" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="N11" s="6" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="O11" s="42" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="P11" s="31"/>
       <c r="Q11" s="31"/>
@@ -6936,23 +6978,23 @@
     </row>
     <row r="12">
       <c r="A12" s="6" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="B12" s="33" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="E12" s="31" t="str">
         <f t="shared" si="1"/>
         <v>dpv:TechnicalOrganisationalMeasure</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="G12" s="31"/>
       <c r="H12" s="31"/>
@@ -6965,13 +7007,13 @@
         <v>44139.0</v>
       </c>
       <c r="M12" s="6" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="N12" s="6" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="O12" s="9" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="P12" s="31"/>
       <c r="Q12" s="31"/>
@@ -6994,24 +7036,45 @@
       <c r="C14" s="44"/>
     </row>
     <row r="15">
+      <c r="A15" s="6" t="s">
+        <v>278</v>
+      </c>
       <c r="C15" s="44"/>
     </row>
     <row r="16">
+      <c r="A16" s="6" t="s">
+        <v>279</v>
+      </c>
       <c r="C16" s="44"/>
     </row>
     <row r="17">
+      <c r="A17" s="6" t="s">
+        <v>280</v>
+      </c>
       <c r="C17" s="44"/>
     </row>
     <row r="18">
+      <c r="A18" s="6" t="s">
+        <v>281</v>
+      </c>
       <c r="C18" s="44"/>
     </row>
     <row r="19">
+      <c r="A19" s="6" t="s">
+        <v>282</v>
+      </c>
       <c r="C19" s="44"/>
     </row>
     <row r="20">
+      <c r="A20" s="6" t="s">
+        <v>283</v>
+      </c>
       <c r="C20" s="44"/>
     </row>
     <row r="21">
+      <c r="A21" s="6" t="s">
+        <v>284</v>
+      </c>
       <c r="C21" s="44"/>
     </row>
     <row r="22">

</xml_diff>

<commit_message>
Provides DPV-DGA extension; fixes GDPR rights html
The DPV-DGA extension is added to the path /dpv/dpv-dga. Implementations
for RDFS+SKOS and OWL are not included. See #62.

The GDPR HTML did not correctly display associated rights for the legal
bases in its table. This has been fixed.
</commit_message>
<xml_diff>
--- a/documentation-generator/vocab_csv/base.xlsx
+++ b/documentation-generator/vocab_csv/base.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="288">
   <si>
     <t>preffix</t>
   </si>
@@ -308,6 +308,15 @@
   </si>
   <si>
     <t>Use-Cases and Requirements for DPV</t>
+  </si>
+  <si>
+    <t>dpv-dga</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/dpv-gda#</t>
+  </si>
+  <si>
+    <t>DGA Extension for DPV</t>
   </si>
   <si>
     <t>dct</t>
@@ -2065,6 +2074,23 @@
         <v>97</v>
       </c>
     </row>
+    <row r="30">
+      <c r="A30" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="D30" s="8">
+        <v>45189.0</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="B2"/>
@@ -2119,8 +2145,9 @@
     <hyperlink r:id="rId50" ref="B27"/>
     <hyperlink r:id="rId51" ref="B28"/>
     <hyperlink r:id="rId52" ref="B29"/>
+    <hyperlink r:id="rId53" ref="B30"/>
   </hyperlinks>
-  <drawing r:id="rId53"/>
+  <drawing r:id="rId54"/>
 </worksheet>
 </file>
 
@@ -2166,13 +2193,13 @@
     </row>
     <row r="2">
       <c r="A2" s="15" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="D2" s="17"/>
       <c r="E2" s="17"/>
@@ -2196,13 +2223,13 @@
     </row>
     <row r="3">
       <c r="A3" s="18" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="17"/>
@@ -2226,13 +2253,13 @@
     </row>
     <row r="4">
       <c r="A4" s="18" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="D4" s="17"/>
       <c r="E4" s="17"/>
@@ -2256,13 +2283,13 @@
     </row>
     <row r="5">
       <c r="A5" s="18" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="D5" s="17"/>
       <c r="E5" s="17"/>
@@ -2286,13 +2313,13 @@
     </row>
     <row r="6">
       <c r="A6" s="18" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="D6" s="17"/>
       <c r="E6" s="17"/>
@@ -2316,13 +2343,13 @@
     </row>
     <row r="7">
       <c r="A7" s="15" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="D7" s="17"/>
       <c r="E7" s="17"/>
@@ -2346,10 +2373,10 @@
     </row>
     <row r="8">
       <c r="A8" s="15" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C8" s="21" t="str">
         <f>HYPERLINK("https://www.specialprivacy.eu/images/documents/SPECIAL_D25_M21_V10.pdf","SPECIAL Log vocabulary cf. SPECIAL Deliverable D2.5")</f>
@@ -2377,13 +2404,13 @@
     </row>
     <row r="9">
       <c r="A9" s="15" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="D9" s="17"/>
       <c r="E9" s="17"/>
@@ -2407,13 +2434,13 @@
     </row>
     <row r="10">
       <c r="A10" s="15" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="D10" s="17"/>
       <c r="E10" s="17"/>
@@ -2437,13 +2464,13 @@
     </row>
     <row r="11">
       <c r="A11" s="23" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="D11" s="17"/>
       <c r="E11" s="17"/>
@@ -2467,13 +2494,13 @@
     </row>
     <row r="12">
       <c r="A12" s="15" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="D12" s="17"/>
       <c r="E12" s="17"/>
@@ -2497,13 +2524,13 @@
     </row>
     <row r="13">
       <c r="A13" s="15" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="D13" s="17"/>
       <c r="E13" s="17"/>
@@ -2527,13 +2554,13 @@
     </row>
     <row r="14">
       <c r="A14" s="23" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D14" s="17"/>
       <c r="E14" s="17"/>
@@ -2557,90 +2584,90 @@
     </row>
     <row r="15">
       <c r="A15" s="6" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="6" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="6" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="6" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="6" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="6" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="6" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="6" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -2696,66 +2723,66 @@
   <sheetData>
     <row r="1" ht="28.5" customHeight="1">
       <c r="A1" s="24" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="C1" s="25" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="D1" s="24" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="E1" s="24" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="F1" s="24" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="G1" s="24" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="H1" s="24" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="I1" s="26" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="J1" s="27" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="L1" s="28" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="6" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -2769,13 +2796,13 @@
         <v>44139.0</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="P2" s="31"/>
       <c r="Q2" s="31"/>
@@ -2797,32 +2824,32 @@
     </row>
     <row r="3">
       <c r="A3" s="6" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="F3" s="6"/>
       <c r="G3" s="6" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="J3" s="13" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="K3" s="8">
         <v>43560.0</v>
@@ -2831,13 +2858,13 @@
         <v>44580.0</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="O3" s="7" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="P3" s="31"/>
       <c r="Q3" s="31"/>
@@ -2859,30 +2886,30 @@
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="6" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="I4" s="31"/>
       <c r="J4" s="13" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="K4" s="8">
         <v>43560.0</v>
@@ -2891,13 +2918,13 @@
         <v>44139.0</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="O4" s="9" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="P4" s="31"/>
       <c r="Q4" s="31"/>
@@ -2919,30 +2946,30 @@
     </row>
     <row r="5">
       <c r="A5" s="6" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="B5" s="33" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="6" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="I5" s="31"/>
       <c r="J5" s="6" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="K5" s="8">
         <v>43560.0</v>
@@ -2951,13 +2978,13 @@
         <v>44139.0</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="O5" s="9" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="P5" s="31"/>
       <c r="Q5" s="31"/>
@@ -2979,32 +3006,32 @@
     </row>
     <row r="6">
       <c r="A6" s="34" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="B6" s="35" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="6" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="I6" s="36" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="K6" s="8">
         <v>43560.0</v>
@@ -3013,13 +3040,13 @@
         <v>44139.0</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="O6" s="9" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="P6" s="31"/>
       <c r="Q6" s="31"/>
@@ -3041,19 +3068,19 @@
     </row>
     <row r="7">
       <c r="A7" s="34" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="B7" s="35" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="F7" s="31"/>
       <c r="G7" s="31"/>
@@ -3067,13 +3094,13 @@
         <v>44139.0</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="N7" s="6" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="O7" s="9" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="P7" s="31"/>
       <c r="Q7" s="31"/>
@@ -3095,25 +3122,25 @@
     </row>
     <row r="8">
       <c r="A8" s="34" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="B8" s="35" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="F8" s="31"/>
       <c r="G8" s="31"/>
       <c r="H8" s="31"/>
       <c r="I8" s="6" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="J8" s="6"/>
       <c r="K8" s="8">
@@ -3123,11 +3150,11 @@
         <v>44139.0</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="N8" s="31"/>
       <c r="O8" s="9" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="P8" s="31"/>
       <c r="Q8" s="31"/>
@@ -3149,28 +3176,28 @@
     </row>
     <row r="9">
       <c r="A9" s="34" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="B9" s="35" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="F9" s="31"/>
       <c r="G9" s="31"/>
       <c r="H9" s="31"/>
       <c r="I9" s="6" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="J9" s="37" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="K9" s="8">
         <v>43560.0</v>
@@ -3179,13 +3206,13 @@
         <v>44139.0</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="N9" s="6" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="O9" s="9" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="P9" s="31"/>
       <c r="Q9" s="31"/>
@@ -3207,28 +3234,28 @@
     </row>
     <row r="10">
       <c r="A10" s="34" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="B10" s="35" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="F10" s="31"/>
       <c r="G10" s="31"/>
       <c r="H10" s="31"/>
       <c r="I10" s="6" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="J10" s="37" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="K10" s="8">
         <v>43560.0</v>
@@ -3237,13 +3264,13 @@
         <v>44139.0</v>
       </c>
       <c r="M10" s="6" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="N10" s="6" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="O10" s="9" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="P10" s="31"/>
       <c r="Q10" s="31"/>
@@ -3265,25 +3292,25 @@
     </row>
     <row r="11">
       <c r="A11" s="38" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="B11" s="39" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="C11" s="38" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="F11" s="40"/>
       <c r="G11" s="40"/>
       <c r="H11" s="40"/>
       <c r="I11" s="38" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="J11" s="38"/>
       <c r="K11" s="41">
@@ -3291,13 +3318,13 @@
       </c>
       <c r="L11" s="41"/>
       <c r="M11" s="38" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="N11" s="38" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="O11" s="42" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="P11" s="40"/>
       <c r="Q11" s="40"/>
@@ -3319,25 +3346,25 @@
     </row>
     <row r="12">
       <c r="A12" s="38" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="B12" s="39" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="C12" s="38" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="D12" s="38" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="E12" s="38" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="F12" s="40"/>
       <c r="G12" s="40"/>
       <c r="H12" s="40"/>
       <c r="I12" s="38" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="J12" s="38"/>
       <c r="K12" s="41">
@@ -3345,13 +3372,13 @@
       </c>
       <c r="L12" s="41"/>
       <c r="M12" s="38" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="N12" s="38" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="O12" s="42" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="P12" s="40"/>
       <c r="Q12" s="40"/>
@@ -3373,25 +3400,25 @@
     </row>
     <row r="13">
       <c r="A13" s="43" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="F13" s="31"/>
       <c r="G13" s="31"/>
       <c r="H13" s="31"/>
       <c r="I13" s="6" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="J13" s="6"/>
       <c r="K13" s="8">
@@ -3399,13 +3426,13 @@
       </c>
       <c r="L13" s="8"/>
       <c r="M13" s="43" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="N13" s="6" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="O13" s="37" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="P13" s="31"/>
       <c r="Q13" s="31"/>
@@ -6404,69 +6431,69 @@
   <sheetData>
     <row r="1" ht="28.5" customHeight="1">
       <c r="A1" s="24" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="C1" s="25" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="D1" s="24" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="E1" s="24" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="F1" s="24" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="G1" s="24" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="H1" s="24" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="J1" s="27" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="34" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="E2" s="34" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="G2" s="31"/>
       <c r="H2" s="31"/>
@@ -6479,13 +6506,13 @@
         <v>44139.0</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="P2" s="31"/>
       <c r="Q2" s="31"/>
@@ -6503,23 +6530,23 @@
     </row>
     <row r="3">
       <c r="A3" s="34" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="B3" s="35" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="E3" s="34" t="str">
         <f t="shared" ref="E3:E12" si="1">CONCATENATE("dpv:",RIGHT(A3,LEN(A3) - 3))</f>
         <v>dpv:DataSubject</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="G3" s="31"/>
       <c r="H3" s="31"/>
@@ -6532,13 +6559,13 @@
         <v>44139.0</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="O3" s="9" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="P3" s="31"/>
       <c r="Q3" s="31"/>
@@ -6556,23 +6583,23 @@
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="E4" s="31" t="str">
         <f t="shared" si="1"/>
         <v>dpv:LegalBasis</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="G4" s="31"/>
       <c r="H4" s="31"/>
@@ -6585,13 +6612,13 @@
         <v>44139.0</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="O4" s="9" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="P4" s="31"/>
       <c r="Q4" s="31"/>
@@ -6609,23 +6636,23 @@
     </row>
     <row r="5">
       <c r="A5" s="6" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="E5" s="6" t="str">
         <f t="shared" si="1"/>
         <v>dpv:PersonalData</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="G5" s="31"/>
       <c r="H5" s="31"/>
@@ -6636,13 +6663,13 @@
       </c>
       <c r="L5" s="8"/>
       <c r="M5" s="6" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="O5" s="37" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="P5" s="31"/>
       <c r="Q5" s="31"/>
@@ -6660,23 +6687,23 @@
     </row>
     <row r="6">
       <c r="A6" s="6" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="E6" s="31" t="str">
         <f t="shared" si="1"/>
         <v>dpv:PersonalDataHandling</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="G6" s="31"/>
       <c r="H6" s="31"/>
@@ -6687,13 +6714,13 @@
       </c>
       <c r="L6" s="31"/>
       <c r="M6" s="6" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="O6" s="9" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="P6" s="31"/>
       <c r="Q6" s="31"/>
@@ -6711,29 +6738,29 @@
     </row>
     <row r="7">
       <c r="A7" s="6" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="B7" s="33" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="E7" s="6" t="str">
         <f t="shared" si="1"/>
         <v>dpv:Processing</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="G7" s="31"/>
       <c r="H7" s="31"/>
       <c r="I7" s="31"/>
       <c r="J7" s="6" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="K7" s="8">
         <v>43559.0</v>
@@ -6742,13 +6769,13 @@
         <v>44139.0</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="N7" s="6" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="O7" s="9" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="P7" s="31"/>
       <c r="Q7" s="31"/>
@@ -6766,29 +6793,29 @@
     </row>
     <row r="8">
       <c r="A8" s="6" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="B8" s="33" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="E8" s="6" t="str">
         <f t="shared" si="1"/>
         <v>dpv:Purpose</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="G8" s="31"/>
       <c r="H8" s="31"/>
       <c r="I8" s="31"/>
       <c r="J8" s="6" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="K8" s="8">
         <v>43559.0</v>
@@ -6797,13 +6824,13 @@
         <v>44139.0</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="N8" s="6" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="O8" s="9" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="P8" s="31"/>
       <c r="Q8" s="31"/>
@@ -6821,29 +6848,29 @@
     </row>
     <row r="9">
       <c r="A9" s="6" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="B9" s="33" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="E9" s="31" t="str">
         <f t="shared" si="1"/>
         <v>dpv:Recipient</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="G9" s="31"/>
       <c r="H9" s="31"/>
       <c r="I9" s="31"/>
       <c r="J9" s="6" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="K9" s="8">
         <v>43559.0</v>
@@ -6852,13 +6879,13 @@
         <v>44139.0</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="N9" s="6" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="O9" s="9" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="P9" s="31"/>
       <c r="Q9" s="31"/>
@@ -6876,23 +6903,23 @@
     </row>
     <row r="10">
       <c r="A10" s="38" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="B10" s="38" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="C10" s="45" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="E10" s="40" t="str">
         <f t="shared" si="1"/>
         <v>dpv:Right</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="G10" s="40"/>
       <c r="H10" s="40"/>
@@ -6903,13 +6930,13 @@
       </c>
       <c r="L10" s="40"/>
       <c r="M10" s="38" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="N10" s="38" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="O10" s="42" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="P10" s="40"/>
       <c r="Q10" s="40"/>
@@ -6927,23 +6954,23 @@
     </row>
     <row r="11">
       <c r="A11" s="6" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="E11" s="31" t="str">
         <f t="shared" si="1"/>
         <v>dpv:Risk</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="G11" s="31"/>
       <c r="H11" s="31"/>
@@ -6954,13 +6981,13 @@
       </c>
       <c r="L11" s="31"/>
       <c r="M11" s="6" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="N11" s="6" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="O11" s="42" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="P11" s="31"/>
       <c r="Q11" s="31"/>
@@ -6978,23 +7005,23 @@
     </row>
     <row r="12">
       <c r="A12" s="6" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="B12" s="33" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="E12" s="31" t="str">
         <f t="shared" si="1"/>
         <v>dpv:TechnicalOrganisationalMeasure</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="G12" s="31"/>
       <c r="H12" s="31"/>
@@ -7007,13 +7034,13 @@
         <v>44139.0</v>
       </c>
       <c r="M12" s="6" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="N12" s="6" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="O12" s="9" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="P12" s="31"/>
       <c r="Q12" s="31"/>
@@ -7037,43 +7064,43 @@
     </row>
     <row r="15">
       <c r="A15" s="6" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="C15" s="44"/>
     </row>
     <row r="16">
       <c r="A16" s="6" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="C16" s="44"/>
     </row>
     <row r="17">
       <c r="A17" s="6" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="C17" s="44"/>
     </row>
     <row r="18">
       <c r="A18" s="6" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="C18" s="44"/>
     </row>
     <row r="19">
       <c r="A19" s="6" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="C19" s="44"/>
     </row>
     <row r="20">
       <c r="A20" s="6" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="C20" s="44"/>
     </row>
     <row r="21">
       <c r="A21" s="6" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="C21" s="44"/>
     </row>

</xml_diff>